<commit_message>
First Successful Run Through
</commit_message>
<xml_diff>
--- a/ConsolidatedSPO06-23.xlsx
+++ b/ConsolidatedSPO06-23.xlsx
@@ -7,6 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Staff Performance Overview" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Consolidated Data" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -489,7 +490,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -887,7 +888,7 @@
       </c>
       <c r="E8" s="6" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F8" s="7" t="n">
@@ -1040,7 +1041,7 @@
       </c>
       <c r="E11" s="6" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F11" s="7" t="n">
@@ -1072,70 +1073,6 @@
       </c>
       <c r="O11" s="7" t="n">
         <v>26.92</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Chrissy Cummings</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>29</v>
-      </c>
-      <c r="C20" t="n">
-        <v>24</v>
-      </c>
-      <c r="D20" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Danielle Mai</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>9</v>
-      </c>
-      <c r="C21" t="n">
-        <v>7</v>
-      </c>
-      <c r="D21" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Jasmine Saiz</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>56</v>
-      </c>
-      <c r="C22" t="n">
-        <v>27</v>
-      </c>
-      <c r="D22" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Karen Trevizo</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>27</v>
-      </c>
-      <c r="C23" t="n">
-        <v>21</v>
-      </c>
-      <c r="D23" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1150,4 +1087,387 @@
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="R2:AT5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2">
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Chrissy Cummings</t>
+        </is>
+      </c>
+      <c r="S2" t="n">
+        <v>3</v>
+      </c>
+      <c r="T2" t="n">
+        <v>3</v>
+      </c>
+      <c r="U2" t="n">
+        <v>1</v>
+      </c>
+      <c r="V2" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="W2" t="n">
+        <v>251</v>
+      </c>
+      <c r="X2" t="n">
+        <v>270.29</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>251</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>270.29</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>83.67</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>90.09999999999999</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>26</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>21</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>1843</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>1985.86</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>1843</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>1985.86</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>70.88</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>76.38</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Danielle Mai</t>
+        </is>
+      </c>
+      <c r="S3" t="n">
+        <v>8</v>
+      </c>
+      <c r="T3" t="n">
+        <v>7</v>
+      </c>
+      <c r="U3" t="n">
+        <v>1</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>571</v>
+      </c>
+      <c r="X3" t="n">
+        <v>614.88</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>21.53</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>591</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>636.41</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>73.88</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>79.55</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>10.78</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>10.78</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>10.78</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Jasmine Saiz</t>
+        </is>
+      </c>
+      <c r="S4" t="n">
+        <v>5</v>
+      </c>
+      <c r="T4" t="n">
+        <v>5</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="W4" t="n">
+        <v>410</v>
+      </c>
+      <c r="X4" t="n">
+        <v>441.51</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>410</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>441.51</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>82</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>88.3</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>51</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>22</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>10</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>3697</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>3983.6</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>3697</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>3983.6</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>72.48999999999999</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>78.11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Karen Trevizo</t>
+        </is>
+      </c>
+      <c r="S5" t="n">
+        <v>19</v>
+      </c>
+      <c r="T5" t="n">
+        <v>18</v>
+      </c>
+      <c r="U5" t="n">
+        <v>1</v>
+      </c>
+      <c r="V5" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="W5" t="n">
+        <v>1376</v>
+      </c>
+      <c r="X5" t="n">
+        <v>1481.76</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>14</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>15.08</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>1390</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>1496.84</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>73.16</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>78.78</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>8</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>580</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>624.96</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>580</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>624.96</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>72.5</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>78.12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
messing with for complete consolidation
</commit_message>
<xml_diff>
--- a/ConsolidatedSPO06-23.xlsx
+++ b/ConsolidatedSPO06-23.xlsx
@@ -1095,7 +1095,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="R2:AT5"/>
+  <dimension ref="A2:AC13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1104,367 +1104,1095 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
-      <c r="R2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>Chrissy Cummings</t>
         </is>
       </c>
+      <c r="B2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="F2" t="n">
+        <v>251</v>
+      </c>
+      <c r="G2" t="n">
+        <v>270.29</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>251</v>
+      </c>
+      <c r="M2" t="n">
+        <v>270.29</v>
+      </c>
+      <c r="N2" t="n">
+        <v>83.67</v>
+      </c>
+      <c r="O2" t="n">
+        <v>90.09999999999999</v>
+      </c>
+      <c r="P2" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>21</v>
+      </c>
+      <c r="R2" t="n">
+        <v>5</v>
+      </c>
       <c r="S2" t="n">
-        <v>3</v>
+        <v>4.8</v>
       </c>
       <c r="T2" t="n">
-        <v>3</v>
+        <v>1843</v>
       </c>
       <c r="U2" t="n">
-        <v>1</v>
+        <v>1985.86</v>
       </c>
       <c r="V2" t="n">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>251</v>
+        <v>0</v>
       </c>
       <c r="X2" t="n">
-        <v>270.29</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="n">
         <v>0</v>
       </c>
       <c r="Z2" t="n">
-        <v>0</v>
+        <v>1843</v>
       </c>
       <c r="AA2" t="n">
-        <v>0</v>
+        <v>1985.86</v>
       </c>
       <c r="AB2" t="n">
-        <v>0</v>
+        <v>70.88</v>
       </c>
       <c r="AC2" t="n">
-        <v>251</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>270.29</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>83.67</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>90.09999999999999</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>26</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>21</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>5</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="AK2" t="n">
-        <v>1843</v>
-      </c>
-      <c r="AL2" t="n">
-        <v>1985.86</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>1843</v>
-      </c>
-      <c r="AR2" t="n">
-        <v>1985.86</v>
-      </c>
-      <c r="AS2" t="n">
-        <v>70.88</v>
-      </c>
-      <c r="AT2" t="n">
         <v>76.38</v>
       </c>
     </row>
     <row r="3">
-      <c r="R3" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>Danielle Mai</t>
         </is>
       </c>
+      <c r="B3" t="n">
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>571</v>
+      </c>
+      <c r="G3" t="n">
+        <v>614.88</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K3" t="n">
+        <v>21.53</v>
+      </c>
+      <c r="L3" t="n">
+        <v>591</v>
+      </c>
+      <c r="M3" t="n">
+        <v>636.41</v>
+      </c>
+      <c r="N3" t="n">
+        <v>73.88</v>
+      </c>
+      <c r="O3" t="n">
+        <v>79.55</v>
+      </c>
+      <c r="P3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
       <c r="S3" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="U3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V3" t="n">
         <v>0</v>
       </c>
       <c r="W3" t="n">
-        <v>571</v>
+        <v>0</v>
       </c>
       <c r="X3" t="n">
-        <v>614.88</v>
+        <v>10</v>
       </c>
       <c r="Y3" t="n">
-        <v>0</v>
+        <v>10.78</v>
       </c>
       <c r="Z3" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AA3" t="n">
-        <v>20</v>
+        <v>10.78</v>
       </c>
       <c r="AB3" t="n">
-        <v>21.53</v>
+        <v>10</v>
       </c>
       <c r="AC3" t="n">
-        <v>591</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>636.41</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>73.88</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>79.55</v>
-      </c>
-      <c r="AG3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO3" t="n">
-        <v>10</v>
-      </c>
-      <c r="AP3" t="n">
-        <v>10.78</v>
-      </c>
-      <c r="AQ3" t="n">
-        <v>10</v>
-      </c>
-      <c r="AR3" t="n">
-        <v>10.78</v>
-      </c>
-      <c r="AS3" t="n">
-        <v>10</v>
-      </c>
-      <c r="AT3" t="n">
         <v>10.78</v>
       </c>
     </row>
     <row r="4">
-      <c r="R4" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>Jasmine Saiz</t>
         </is>
       </c>
+      <c r="B4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="F4" t="n">
+        <v>410</v>
+      </c>
+      <c r="G4" t="n">
+        <v>441.51</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>410</v>
+      </c>
+      <c r="M4" t="n">
+        <v>441.51</v>
+      </c>
+      <c r="N4" t="n">
+        <v>82</v>
+      </c>
+      <c r="O4" t="n">
+        <v>88.3</v>
+      </c>
+      <c r="P4" t="n">
+        <v>51</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>22</v>
+      </c>
+      <c r="R4" t="n">
+        <v>10</v>
+      </c>
       <c r="S4" t="n">
-        <v>5</v>
+        <v>4.9</v>
       </c>
       <c r="T4" t="n">
-        <v>5</v>
+        <v>3697</v>
       </c>
       <c r="U4" t="n">
-        <v>0</v>
+        <v>3983.6</v>
       </c>
       <c r="V4" t="n">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>410</v>
+        <v>0</v>
       </c>
       <c r="X4" t="n">
-        <v>441.51</v>
+        <v>0</v>
       </c>
       <c r="Y4" t="n">
         <v>0</v>
       </c>
       <c r="Z4" t="n">
-        <v>0</v>
+        <v>3697</v>
       </c>
       <c r="AA4" t="n">
-        <v>0</v>
+        <v>3983.6</v>
       </c>
       <c r="AB4" t="n">
-        <v>0</v>
+        <v>72.48999999999999</v>
       </c>
       <c r="AC4" t="n">
-        <v>410</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>441.51</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>82</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>88.3</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>51</v>
-      </c>
-      <c r="AH4" t="n">
-        <v>22</v>
-      </c>
-      <c r="AI4" t="n">
-        <v>10</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="AK4" t="n">
-        <v>3697</v>
-      </c>
-      <c r="AL4" t="n">
-        <v>3983.6</v>
-      </c>
-      <c r="AM4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ4" t="n">
-        <v>3697</v>
-      </c>
-      <c r="AR4" t="n">
-        <v>3983.6</v>
-      </c>
-      <c r="AS4" t="n">
-        <v>72.48999999999999</v>
-      </c>
-      <c r="AT4" t="n">
         <v>78.11</v>
       </c>
     </row>
     <row r="5">
-      <c r="R5" t="inlineStr">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Justyne Martinez </t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>25</v>
+      </c>
+      <c r="C5" t="n">
+        <v>15</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1762.5</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1897.93</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>10</v>
+      </c>
+      <c r="K5" t="n">
+        <v>10.77</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1772.5</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1908.7</v>
+      </c>
+      <c r="N5" t="n">
+        <v>70.90000000000001</v>
+      </c>
+      <c r="O5" t="n">
+        <v>76.34999999999999</v>
+      </c>
+      <c r="P5" t="n">
+        <v/>
+      </c>
+      <c r="Q5" t="n">
+        <v/>
+      </c>
+      <c r="R5" t="n">
+        <v/>
+      </c>
+      <c r="S5" t="n">
+        <v/>
+      </c>
+      <c r="T5" t="n">
+        <v/>
+      </c>
+      <c r="U5" t="n">
+        <v/>
+      </c>
+      <c r="V5" t="n">
+        <v/>
+      </c>
+      <c r="W5" t="n">
+        <v/>
+      </c>
+      <c r="X5" t="n">
+        <v/>
+      </c>
+      <c r="Y5" t="n">
+        <v/>
+      </c>
+      <c r="Z5" t="n">
+        <v/>
+      </c>
+      <c r="AA5" t="n">
+        <v/>
+      </c>
+      <c r="AB5" t="n">
+        <v/>
+      </c>
+      <c r="AC5" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
           <t>Karen Trevizo</t>
         </is>
       </c>
-      <c r="S5" t="n">
+      <c r="B6" t="n">
         <v>19</v>
       </c>
-      <c r="T5" t="n">
+      <c r="C6" t="n">
         <v>18</v>
       </c>
-      <c r="U5" t="n">
+      <c r="D6" t="n">
         <v>1</v>
       </c>
-      <c r="V5" t="n">
+      <c r="E6" t="n">
         <v>4.6</v>
       </c>
-      <c r="W5" t="n">
+      <c r="F6" t="n">
         <v>1376</v>
       </c>
-      <c r="X5" t="n">
+      <c r="G6" t="n">
         <v>1481.76</v>
       </c>
-      <c r="Y5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA5" t="n">
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
         <v>14</v>
       </c>
-      <c r="AB5" t="n">
+      <c r="K6" t="n">
         <v>15.08</v>
       </c>
-      <c r="AC5" t="n">
+      <c r="L6" t="n">
         <v>1390</v>
       </c>
-      <c r="AD5" t="n">
+      <c r="M6" t="n">
         <v>1496.84</v>
       </c>
-      <c r="AE5" t="n">
+      <c r="N6" t="n">
         <v>73.16</v>
       </c>
-      <c r="AF5" t="n">
+      <c r="O6" t="n">
         <v>78.78</v>
       </c>
-      <c r="AG5" t="n">
+      <c r="P6" t="n">
         <v>8</v>
       </c>
-      <c r="AH5" t="n">
+      <c r="Q6" t="n">
         <v>3</v>
       </c>
-      <c r="AI5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ5" t="n">
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
         <v>4.8</v>
       </c>
-      <c r="AK5" t="n">
+      <c r="T6" t="n">
         <v>580</v>
       </c>
-      <c r="AL5" t="n">
+      <c r="U6" t="n">
         <v>624.96</v>
       </c>
-      <c r="AM5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ5" t="n">
+      <c r="V6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="n">
         <v>580</v>
       </c>
-      <c r="AR5" t="n">
+      <c r="AA6" t="n">
         <v>624.96</v>
       </c>
-      <c r="AS5" t="n">
+      <c r="AB6" t="n">
         <v>72.5</v>
       </c>
-      <c r="AT5" t="n">
+      <c r="AC6" t="n">
         <v>78.12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Maggie  Farrell</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>38</v>
+      </c>
+      <c r="C7" t="n">
+        <v>20</v>
+      </c>
+      <c r="D7" t="n">
+        <v>4</v>
+      </c>
+      <c r="E7" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2569.85</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2767.35</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>20</v>
+      </c>
+      <c r="K7" t="n">
+        <v>21.54</v>
+      </c>
+      <c r="L7" t="n">
+        <v>2589.85</v>
+      </c>
+      <c r="M7" t="n">
+        <v>2788.89</v>
+      </c>
+      <c r="N7" t="n">
+        <v>68.15000000000001</v>
+      </c>
+      <c r="O7" t="n">
+        <v>73.39</v>
+      </c>
+      <c r="P7" t="n">
+        <v/>
+      </c>
+      <c r="Q7" t="n">
+        <v/>
+      </c>
+      <c r="R7" t="n">
+        <v/>
+      </c>
+      <c r="S7" t="n">
+        <v/>
+      </c>
+      <c r="T7" t="n">
+        <v/>
+      </c>
+      <c r="U7" t="n">
+        <v/>
+      </c>
+      <c r="V7" t="n">
+        <v/>
+      </c>
+      <c r="W7" t="n">
+        <v/>
+      </c>
+      <c r="X7" t="n">
+        <v/>
+      </c>
+      <c r="Y7" t="n">
+        <v/>
+      </c>
+      <c r="Z7" t="n">
+        <v/>
+      </c>
+      <c r="AA7" t="n">
+        <v/>
+      </c>
+      <c r="AB7" t="n">
+        <v/>
+      </c>
+      <c r="AC7" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Makayla Baca</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>24</v>
+      </c>
+      <c r="C8" t="n">
+        <v>7</v>
+      </c>
+      <c r="D8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1750</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1884.49</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>30</v>
+      </c>
+      <c r="K8" t="n">
+        <v>32.31</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1780</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1916.8</v>
+      </c>
+      <c r="N8" t="n">
+        <v>74.17</v>
+      </c>
+      <c r="O8" t="n">
+        <v>79.87</v>
+      </c>
+      <c r="P8" t="n">
+        <v/>
+      </c>
+      <c r="Q8" t="n">
+        <v/>
+      </c>
+      <c r="R8" t="n">
+        <v/>
+      </c>
+      <c r="S8" t="n">
+        <v/>
+      </c>
+      <c r="T8" t="n">
+        <v/>
+      </c>
+      <c r="U8" t="n">
+        <v/>
+      </c>
+      <c r="V8" t="n">
+        <v/>
+      </c>
+      <c r="W8" t="n">
+        <v/>
+      </c>
+      <c r="X8" t="n">
+        <v/>
+      </c>
+      <c r="Y8" t="n">
+        <v/>
+      </c>
+      <c r="Z8" t="n">
+        <v/>
+      </c>
+      <c r="AA8" t="n">
+        <v/>
+      </c>
+      <c r="AB8" t="n">
+        <v/>
+      </c>
+      <c r="AC8" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Matthew Young</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>25</v>
+      </c>
+      <c r="G9" t="n">
+        <v>26.92</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>25</v>
+      </c>
+      <c r="M9" t="n">
+        <v>26.92</v>
+      </c>
+      <c r="N9" t="n">
+        <v>25</v>
+      </c>
+      <c r="O9" t="n">
+        <v>26.92</v>
+      </c>
+      <c r="P9" t="n">
+        <v/>
+      </c>
+      <c r="Q9" t="n">
+        <v/>
+      </c>
+      <c r="R9" t="n">
+        <v/>
+      </c>
+      <c r="S9" t="n">
+        <v/>
+      </c>
+      <c r="T9" t="n">
+        <v/>
+      </c>
+      <c r="U9" t="n">
+        <v/>
+      </c>
+      <c r="V9" t="n">
+        <v/>
+      </c>
+      <c r="W9" t="n">
+        <v/>
+      </c>
+      <c r="X9" t="n">
+        <v/>
+      </c>
+      <c r="Y9" t="n">
+        <v/>
+      </c>
+      <c r="Z9" t="n">
+        <v/>
+      </c>
+      <c r="AA9" t="n">
+        <v/>
+      </c>
+      <c r="AB9" t="n">
+        <v/>
+      </c>
+      <c r="AC9" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Vy Torino</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>17</v>
+      </c>
+      <c r="C10" t="n">
+        <v>6</v>
+      </c>
+      <c r="D10" t="n">
+        <v>6</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1406</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1514.04</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1406</v>
+      </c>
+      <c r="M10" t="n">
+        <v>1514.04</v>
+      </c>
+      <c r="N10" t="n">
+        <v>82.70999999999999</v>
+      </c>
+      <c r="O10" t="n">
+        <v>89.06</v>
+      </c>
+      <c r="P10" t="n">
+        <v/>
+      </c>
+      <c r="Q10" t="n">
+        <v/>
+      </c>
+      <c r="R10" t="n">
+        <v/>
+      </c>
+      <c r="S10" t="n">
+        <v/>
+      </c>
+      <c r="T10" t="n">
+        <v/>
+      </c>
+      <c r="U10" t="n">
+        <v/>
+      </c>
+      <c r="V10" t="n">
+        <v/>
+      </c>
+      <c r="W10" t="n">
+        <v/>
+      </c>
+      <c r="X10" t="n">
+        <v/>
+      </c>
+      <c r="Y10" t="n">
+        <v/>
+      </c>
+      <c r="Z10" t="n">
+        <v/>
+      </c>
+      <c r="AA10" t="n">
+        <v/>
+      </c>
+      <c r="AB10" t="n">
+        <v/>
+      </c>
+      <c r="AC10" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Aminah Avalos</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v/>
+      </c>
+      <c r="C11" t="n">
+        <v/>
+      </c>
+      <c r="D11" t="n">
+        <v/>
+      </c>
+      <c r="E11" t="n">
+        <v/>
+      </c>
+      <c r="F11" t="n">
+        <v/>
+      </c>
+      <c r="G11" t="n">
+        <v/>
+      </c>
+      <c r="H11" t="n">
+        <v/>
+      </c>
+      <c r="I11" t="n">
+        <v/>
+      </c>
+      <c r="J11" t="n">
+        <v/>
+      </c>
+      <c r="K11" t="n">
+        <v/>
+      </c>
+      <c r="L11" t="n">
+        <v/>
+      </c>
+      <c r="M11" t="n">
+        <v/>
+      </c>
+      <c r="N11" t="n">
+        <v/>
+      </c>
+      <c r="O11" t="n">
+        <v/>
+      </c>
+      <c r="P11" t="n">
+        <v>34</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>14</v>
+      </c>
+      <c r="R11" t="n">
+        <v>8</v>
+      </c>
+      <c r="S11" t="n">
+        <v>5</v>
+      </c>
+      <c r="T11" t="n">
+        <v>2781</v>
+      </c>
+      <c r="U11" t="n">
+        <v>2996.59</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>2781</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>2996.59</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>81.79000000000001</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>88.14</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Izzy Kruis</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v/>
+      </c>
+      <c r="C12" t="n">
+        <v/>
+      </c>
+      <c r="D12" t="n">
+        <v/>
+      </c>
+      <c r="E12" t="n">
+        <v/>
+      </c>
+      <c r="F12" t="n">
+        <v/>
+      </c>
+      <c r="G12" t="n">
+        <v/>
+      </c>
+      <c r="H12" t="n">
+        <v/>
+      </c>
+      <c r="I12" t="n">
+        <v/>
+      </c>
+      <c r="J12" t="n">
+        <v/>
+      </c>
+      <c r="K12" t="n">
+        <v/>
+      </c>
+      <c r="L12" t="n">
+        <v/>
+      </c>
+      <c r="M12" t="n">
+        <v/>
+      </c>
+      <c r="N12" t="n">
+        <v/>
+      </c>
+      <c r="O12" t="n">
+        <v/>
+      </c>
+      <c r="P12" t="n">
+        <v>44</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>24</v>
+      </c>
+      <c r="R12" t="n">
+        <v>6</v>
+      </c>
+      <c r="S12" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="T12" t="n">
+        <v>2790</v>
+      </c>
+      <c r="U12" t="n">
+        <v>3006.26</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0</v>
+      </c>
+      <c r="X12" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>16.7</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>2805.5</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>3022.96</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>63.76</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>68.7</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Krisdee Martinez</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v/>
+      </c>
+      <c r="C13" t="n">
+        <v/>
+      </c>
+      <c r="D13" t="n">
+        <v/>
+      </c>
+      <c r="E13" t="n">
+        <v/>
+      </c>
+      <c r="F13" t="n">
+        <v/>
+      </c>
+      <c r="G13" t="n">
+        <v/>
+      </c>
+      <c r="H13" t="n">
+        <v/>
+      </c>
+      <c r="I13" t="n">
+        <v/>
+      </c>
+      <c r="J13" t="n">
+        <v/>
+      </c>
+      <c r="K13" t="n">
+        <v/>
+      </c>
+      <c r="L13" t="n">
+        <v/>
+      </c>
+      <c r="M13" t="n">
+        <v/>
+      </c>
+      <c r="N13" t="n">
+        <v/>
+      </c>
+      <c r="O13" t="n">
+        <v/>
+      </c>
+      <c r="P13" t="n">
+        <v>39</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>19</v>
+      </c>
+      <c r="R13" t="n">
+        <v>10</v>
+      </c>
+      <c r="S13" t="n">
+        <v>5</v>
+      </c>
+      <c r="T13" t="n">
+        <v>2542.8</v>
+      </c>
+      <c r="U13" t="n">
+        <v>2739.92</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" t="n">
+        <v>0</v>
+      </c>
+      <c r="X13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>2542.8</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>2739.92</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>65.2</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>70.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>